<commit_message>
salvataggio query utente su file excel
</commit_message>
<xml_diff>
--- a/src/main/resources/reportUtenteTemplate.xlsx
+++ b/src/main/resources/reportUtenteTemplate.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emicovi/Documents/workspace/nanosoft_MechAdvisor/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE765AB-CA4A-6340-94B5-361291AE3DC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A60626D5-20D6-9144-8C4C-51B247A97FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="query3" sheetId="1" r:id="rId1"/>
+    <sheet name="Foglio1" sheetId="2" r:id="rId1"/>
+    <sheet name="Foglio2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
   <si>
     <t>Nome</t>
   </si>
@@ -393,18 +394,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D327A8B-396E-AC4E-86E3-85D84A0BA8B2}">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="31.1640625" customWidth="1"/>
-    <col min="2" max="2" width="47.83203125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCD70F9D-7DD6-A943-933C-91F780327E84}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">

</xml_diff>